<commit_message>
Add comments for the spreadsheet file, update the README file.
</commit_message>
<xml_diff>
--- a/create_form.xlsx
+++ b/create_form.xlsx
@@ -1,13 +1,202 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="20490" windowHeight="7800"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>lucky</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Quiz title</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Quiz description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Questions</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Answer options</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Correct answer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Point for each question.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Section separator</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>lucky:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Section separator</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -154,85 +343,439 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="26">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="7">
-    <border/>
+  <borders count="15">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -241,72 +784,380 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -496,23 +1347,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="45.29"/>
+    <col min="1" max="1" width="45.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="12.75" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="12.75" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,7 +1389,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" ht="12.75" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -544,7 +1399,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" ht="12.75" spans="1:8">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -554,223 +1409,225 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+    <row r="5" ht="12.75" spans="1:8">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
+    <row r="6" ht="12.75" spans="1:8">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="14">
-        <v>1.0</v>
+      <c r="H6" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
+    <row r="7" ht="12.75" spans="1:8">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="14">
-        <v>1.0</v>
+      <c r="H7" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="13" t="s">
+    <row r="8" ht="12.75" spans="1:8">
+      <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14">
-        <v>1.0</v>
+      <c r="H8" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="14" t="s">
+    <row r="9" ht="12.75" spans="1:8">
+      <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
-    <row r="10">
-      <c r="A10" s="13" t="s">
+    <row r="10" ht="12.75" spans="1:8">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14">
-        <v>1.0</v>
+      <c r="H10" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="13" t="s">
+    <row r="11" ht="12.75" spans="1:8">
+      <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="14">
-        <v>1.0</v>
+      <c r="H11" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="14" t="s">
+    <row r="12" ht="12.75" spans="1:8">
+      <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
-    <row r="13">
-      <c r="A13" s="14" t="s">
+    <row r="13" ht="12.75" spans="1:8">
+      <c r="A13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14">
-        <v>2.0</v>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12">
+        <v>2</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="14" t="s">
+    <row r="14" ht="12.75" spans="1:8">
+      <c r="A14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="14">
-        <v>3.0</v>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>